<commit_message>
restore from cifar pretrain and resize,using batch_size=128.
</commit_message>
<xml_diff>
--- a/result0523.xlsx
+++ b/result0523.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="80">
   <si>
     <t>No</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>exp13</t>
+  </si>
+  <si>
+    <t>exp14</t>
   </si>
   <si>
     <t>Check RNN-demb=50</t>
@@ -356,10 +359,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V30"/>
+  <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T13" activeCellId="0" sqref="T13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1066,6 +1069,9 @@
       <c r="A16" s="0" t="s">
         <v>71</v>
       </c>
+      <c r="K16" s="0" t="s">
+        <v>50</v>
+      </c>
       <c r="N16" s="0" t="n">
         <v>10</v>
       </c>
@@ -1086,6 +1092,9 @@
       <c r="A17" s="0" t="s">
         <v>72</v>
       </c>
+      <c r="K17" s="0" t="s">
+        <v>50</v>
+      </c>
       <c r="N17" s="0" t="n">
         <v>30</v>
       </c>
@@ -1106,74 +1115,27 @@
       <c r="A18" s="0" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="K18" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="0" t="s">
+      <c r="K19" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>0.629</v>
+      </c>
+      <c r="P19" s="0" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>76</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="G21" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="H21" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I21" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K21" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="G22" s="0" t="n">
-        <v>512</v>
-      </c>
-      <c r="H22" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I22" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K22" s="0" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1181,10 +1143,10 @@
         <v>21</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E23" s="0" t="s">
         <v>24</v>
@@ -1205,7 +1167,7 @@
         <v>1</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1213,10 +1175,10 @@
         <v>21</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E24" s="0" t="s">
         <v>24</v>
@@ -1237,76 +1199,76 @@
         <v>1</v>
       </c>
       <c r="K24" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="0" t="n">
         <v>50</v>
       </c>
+      <c r="G25" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I25" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J25" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="B26" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="0" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="G27" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="H27" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I27" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J27" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>36</v>
+      <c r="E26" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>100</v>
-      </c>
-      <c r="G28" s="0" t="n">
-        <v>512</v>
-      </c>
-      <c r="H28" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I28" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J28" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K28" s="0" t="s">
-        <v>36</v>
+      <c r="A28" s="0" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1314,10 +1276,10 @@
         <v>21</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E29" s="0" t="s">
         <v>24</v>
@@ -1338,7 +1300,7 @@
         <v>1</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1346,10 +1308,10 @@
         <v>21</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E30" s="0" t="s">
         <v>24</v>
@@ -1370,6 +1332,70 @@
         <v>1</v>
       </c>
       <c r="K30" s="0" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E31" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G31" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="H31" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I31" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J31" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K31" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>512</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K32" s="0" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tfbaseline_fixqrestore.py.img features are very sparse.
</commit_message>
<xml_diff>
--- a/result0523.xlsx
+++ b/result0523.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="86">
   <si>
     <t>No</t>
   </si>
@@ -245,13 +245,31 @@
     <t>exp14</t>
   </si>
   <si>
+    <t>RNN</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Train not powerful enough</t>
+  </si>
+  <si>
+    <t>50 epoch used 10 min</t>
+  </si>
+  <si>
+    <t>get 4w </t>
+  </si>
+  <si>
+    <t>E0</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>E34</t>
+  </si>
+  <si>
     <t>Check RNN-demb=50</t>
-  </si>
-  <si>
-    <t>RNN</t>
-  </si>
-  <si>
-    <t>F</t>
   </si>
   <si>
     <t>Check RNN-demb=100</t>
@@ -359,10 +377,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L42" activeCellId="0" sqref="L42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1133,269 +1151,456 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F34" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I34" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L34" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M34" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O34" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P34" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q34" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R34" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S34" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="T34" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="0" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="0" t="s">
+      <c r="D37" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="E37" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="T37" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="0" t="n">
+      <c r="V37" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K39" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="H23" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I23" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K23" s="0" t="s">
+      <c r="O39" s="0" t="n">
+        <v>0.666</v>
+      </c>
+      <c r="P39" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="S39" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="L40" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="O40" s="0" t="n">
+        <v>0.699</v>
+      </c>
+      <c r="P40" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" s="0" t="n">
+        <v>4800</v>
+      </c>
+      <c r="H41" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I41" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J41" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K41" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="L41" s="0" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D44" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="E44" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="G44" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="H44" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I44" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J44" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K44" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="0" t="s">
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D45" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="0" t="n">
+      <c r="E45" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F45" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G45" s="0" t="n">
         <v>512</v>
       </c>
-      <c r="H24" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I24" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J24" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K24" s="0" t="s">
+      <c r="H45" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I45" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J45" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K45" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="0" t="s">
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D46" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F25" s="0" t="n">
+      <c r="E46" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F46" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="G25" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="H25" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I25" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J25" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K25" s="0" t="s">
+      <c r="G46" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="H46" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I46" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J46" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K46" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="0" t="s">
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B47" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D47" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="0" t="n">
+      <c r="E47" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="0" t="n">
         <v>50</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G47" s="0" t="n">
         <v>512</v>
       </c>
-      <c r="H26" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I26" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J26" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K26" s="0" t="s">
+      <c r="H47" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I47" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J47" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K47" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="0" t="s">
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B50" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D50" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E29" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29" s="0" t="n">
+      <c r="E50" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="G29" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="H29" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I29" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J29" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K29" s="0" t="s">
+      <c r="G50" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="H50" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I50" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J50" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K50" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="0" t="s">
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B51" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D51" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E30" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F30" s="0" t="n">
+      <c r="E51" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="G30" s="0" t="n">
+      <c r="G51" s="0" t="n">
         <v>512</v>
       </c>
-      <c r="H30" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I30" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J30" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K30" s="0" t="s">
+      <c r="H51" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I51" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J51" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K51" s="0" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" s="0" t="s">
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B52" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D52" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="0" t="n">
+      <c r="E52" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="G31" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="H31" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I31" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J31" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K31" s="0" t="s">
+      <c r="G52" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="H52" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I52" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K52" s="0" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="C32" s="0" t="s">
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B53" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="D53" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" s="0" t="n">
+      <c r="E53" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F53" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="G32" s="0" t="n">
+      <c r="G53" s="0" t="n">
         <v>512</v>
       </c>
-      <c r="H32" s="0" t="n">
-        <v>256</v>
-      </c>
-      <c r="I32" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J32" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K32" s="0" t="s">
+      <c r="H53" s="0" t="n">
+        <v>256</v>
+      </c>
+      <c r="I53" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="J53" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K53" s="0" t="s">
         <v>50</v>
       </c>
     </row>

</xml_diff>